<commit_message>
cm03 - exercise completed
</commit_message>
<xml_diff>
--- a/Golden_Record_Exercise.xlsx
+++ b/Golden_Record_Exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitsharma/Desktop/ML/09_Udacity/06-Udacity_Data_Architect/Project_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7123C4-6CF9-9B4B-BD20-D74769898C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53808BDA-CCCA-754D-BDA7-2DF415140BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="940" windowWidth="27640" windowHeight="15960" activeTab="1" xr2:uid="{409C4832-223E-DA4F-9FFD-14ABC3290AC6}"/>
+    <workbookView xWindow="740" yWindow="940" windowWidth="27640" windowHeight="15960" xr2:uid="{409C4832-223E-DA4F-9FFD-14ABC3290AC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Golden rule format" sheetId="2" r:id="rId1"/>
@@ -1220,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F29826-7F2E-F142-9F70-99F126B848CC}">
   <dimension ref="A1:G469"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15:J61"/>
     </sheetView>
   </sheetViews>
@@ -5643,7 +5643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333EDD88-6D69-744D-83E2-3893DCEB5FCD}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>